<commit_message>
Kiểm tra, sửa lỗi theo phân công
Kiểm tra, sửa lỗi theo phân công
</commit_message>
<xml_diff>
--- a/plan/kehoachphancong_tuan3.xlsx
+++ b/plan/kehoachphancong_tuan3.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\comeh\Documents\GitHub\thanhsang\Do_An_Quan_Ly_Phong_Game\plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\comeh\Documents\GitHub\dotranhaison\Do_An_Quan_Ly_Phong_Game\plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C11701-BFB1-46DB-B279-AC170EA8EB39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E535511C-7BC7-4E1C-B3D9-BA6B12B61382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{322190C4-C314-4CD5-BEB2-F2D9B770BCD3}"/>
   </bookViews>
@@ -411,6 +411,18 @@
     <xf numFmtId="164" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -424,18 +436,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2087,7 +2087,7 @@
   <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2098,204 +2098,204 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="18"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="18"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
+      <c r="A6" s="18"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
+      <c r="A7" s="18"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="18"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
+      <c r="A8" s="18"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="18"/>
     </row>
     <row r="9" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="17" t="s">
+      <c r="C9" s="20"/>
+      <c r="D9" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="18" t="s">
+      <c r="E9" s="20"/>
+      <c r="F9" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="18"/>
-      <c r="H9" s="17" t="s">
+      <c r="G9" s="22"/>
+      <c r="H9" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="16"/>
-      <c r="J9" s="18" t="s">
+      <c r="I9" s="20"/>
+      <c r="J9" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="18"/>
-      <c r="L9" s="17" t="s">
+      <c r="K9" s="22"/>
+      <c r="L9" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="M9" s="16"/>
-      <c r="N9" s="17" t="s">
+      <c r="M9" s="20"/>
+      <c r="N9" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="O9" s="18"/>
+      <c r="O9" s="22"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="21">
+      <c r="B10" s="16">
         <v>44814</v>
       </c>
-      <c r="C10" s="22"/>
-      <c r="D10" s="19">
+      <c r="C10" s="17"/>
+      <c r="D10" s="14">
         <v>44844</v>
       </c>
-      <c r="E10" s="22"/>
-      <c r="F10" s="20">
+      <c r="E10" s="17"/>
+      <c r="F10" s="15">
         <v>44875</v>
       </c>
-      <c r="G10" s="20"/>
-      <c r="H10" s="19">
+      <c r="G10" s="15"/>
+      <c r="H10" s="14">
         <v>44905</v>
       </c>
-      <c r="I10" s="22"/>
-      <c r="J10" s="20" t="s">
+      <c r="I10" s="17"/>
+      <c r="J10" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="K10" s="20"/>
-      <c r="L10" s="19" t="s">
+      <c r="K10" s="15"/>
+      <c r="L10" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="M10" s="22"/>
-      <c r="N10" s="19" t="s">
+      <c r="M10" s="17"/>
+      <c r="N10" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="O10" s="20"/>
+      <c r="O10" s="15"/>
     </row>
     <row r="11" spans="1:15" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
@@ -2377,7 +2377,9 @@
       <c r="B14" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="11"/>
+      <c r="C14" s="11">
+        <v>1</v>
+      </c>
       <c r="D14" s="12"/>
       <c r="E14" s="13"/>
       <c r="F14" s="10"/>
@@ -2398,7 +2400,9 @@
       <c r="B15" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="11"/>
+      <c r="C15" s="11">
+        <v>0</v>
+      </c>
       <c r="D15" s="12"/>
       <c r="E15" s="13"/>
       <c r="F15" s="10"/>
@@ -2635,13 +2639,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="L10:M10"/>
     <mergeCell ref="A1:O8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="D9:E9"/>
@@ -2650,6 +2647,13 @@
     <mergeCell ref="J9:K9"/>
     <mergeCell ref="L9:M9"/>
     <mergeCell ref="N9:O9"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="L10:M10"/>
   </mergeCells>
   <dataValidations count="10">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Nhập ngày đầu tiên trong tuần đối với lịch biểu việc nhà." sqref="B10" xr:uid="{3049090B-60E9-4942-8275-FDD8077FACF7}"/>

</xml_diff>

<commit_message>
kiem tra lan cuoi
kiem tra lan cuoi
</commit_message>
<xml_diff>
--- a/plan/kehoachphancong_tuan3.xlsx
+++ b/plan/kehoachphancong_tuan3.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\comeh\Documents\GitHub\dotranhaison\Do_An_Quan_Ly_Phong_Game\plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\comeh\Documents\GitHub\Do_An_Quan_Ly_Phong_Game\plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E535511C-7BC7-4E1C-B3D9-BA6B12B61382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{207BC753-A5F0-42E8-8C0E-6A9576DFBA45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{322190C4-C314-4CD5-BEB2-F2D9B770BCD3}"/>
   </bookViews>
@@ -411,18 +411,6 @@
     <xf numFmtId="164" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -436,6 +424,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2087,7 +2087,7 @@
   <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2098,204 +2098,204 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="18"/>
-      <c r="O3" s="18"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
-      <c r="N4" s="18"/>
-      <c r="O4" s="18"/>
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="18"/>
-      <c r="O5" s="18"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="18"/>
-      <c r="O6" s="18"/>
+      <c r="A6" s="14"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
+      <c r="A7" s="14"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
-      <c r="O8" s="18"/>
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
     </row>
     <row r="9" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="21" t="s">
+      <c r="C9" s="16"/>
+      <c r="D9" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="20"/>
-      <c r="F9" s="22" t="s">
+      <c r="E9" s="16"/>
+      <c r="F9" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="22"/>
-      <c r="H9" s="21" t="s">
+      <c r="G9" s="18"/>
+      <c r="H9" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="20"/>
-      <c r="J9" s="22" t="s">
+      <c r="I9" s="16"/>
+      <c r="J9" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="22"/>
-      <c r="L9" s="21" t="s">
+      <c r="K9" s="18"/>
+      <c r="L9" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="M9" s="20"/>
-      <c r="N9" s="21" t="s">
+      <c r="M9" s="16"/>
+      <c r="N9" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="O9" s="22"/>
+      <c r="O9" s="18"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="16">
+      <c r="B10" s="21">
         <v>44814</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="14">
+      <c r="C10" s="22"/>
+      <c r="D10" s="19">
         <v>44844</v>
       </c>
-      <c r="E10" s="17"/>
-      <c r="F10" s="15">
+      <c r="E10" s="22"/>
+      <c r="F10" s="20">
         <v>44875</v>
       </c>
-      <c r="G10" s="15"/>
-      <c r="H10" s="14">
+      <c r="G10" s="20"/>
+      <c r="H10" s="19">
         <v>44905</v>
       </c>
-      <c r="I10" s="17"/>
-      <c r="J10" s="15" t="s">
+      <c r="I10" s="22"/>
+      <c r="J10" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="K10" s="15"/>
-      <c r="L10" s="14" t="s">
+      <c r="K10" s="20"/>
+      <c r="L10" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="M10" s="17"/>
-      <c r="N10" s="14" t="s">
+      <c r="M10" s="22"/>
+      <c r="N10" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="O10" s="15"/>
+      <c r="O10" s="20"/>
     </row>
     <row r="11" spans="1:15" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
@@ -2401,7 +2401,7 @@
         <v>4</v>
       </c>
       <c r="C15" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="13"/>
@@ -2639,6 +2639,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="L10:M10"/>
     <mergeCell ref="A1:O8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="D9:E9"/>
@@ -2647,13 +2654,6 @@
     <mergeCell ref="J9:K9"/>
     <mergeCell ref="L9:M9"/>
     <mergeCell ref="N9:O9"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="L10:M10"/>
   </mergeCells>
   <dataValidations count="10">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Nhập ngày đầu tiên trong tuần đối với lịch biểu việc nhà." sqref="B10" xr:uid="{3049090B-60E9-4942-8275-FDD8077FACF7}"/>

</xml_diff>

<commit_message>
cập nhật kế hoạch phân công tuần 3 (10/10/22)
cập nhật kế hoạch phân công tuần 3 (10/10/22)
</commit_message>
<xml_diff>
--- a/plan/kehoachphancong_tuan3.xlsx
+++ b/plan/kehoachphancong_tuan3.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\comeh\Documents\GitHub\Do_An_Quan_Ly_Phong_Game\plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{207BC753-A5F0-42E8-8C0E-6A9576DFBA45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{322190C4-C314-4CD5-BEB2-F2D9B770BCD3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770"/>
   </bookViews>
   <sheets>
     <sheet name="Trang_tính1" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
   <definedNames>
     <definedName name="Ngày_đầu_tiên">Trang_tính1!$C$3</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>KẾ HOẠCH PHÂN CÔNG HÀNG TUẦN</t>
   </si>
@@ -101,7 +100,17 @@
     <t>- Kiểm tra lần cuối và gộp vào nhánh chính</t>
   </si>
   <si>
-    <t xml:space="preserve">- Viết code khai báo biến ThueMotMay với struct, thông tin mỗi máy tính như sau:
+    <t>- Từ tác vụ đầu tiên của Xuân Sang
+    + Viết thêm hàm đọc/ghi một người thuê từ file/ra file
+[Bổ sung]
++ Viết thêm hàm thayDoiThongTinTaiKhoanMatKhau()</t>
+  </si>
+  <si>
+    <t>Xuân Lam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Tạo mới và viết vào file ThueMotMay.hpp]
+- Viết code khai báo biến ThueMotMay với struct, thông tin mỗi máy tính như sau:
     + Tài khoản (char[30])
     + Mật khẩu (char[30])
     + Số điện thoại (char[15])
@@ -115,16 +124,47 @@
 </t>
   </si>
   <si>
-    <t>- Từ tác vụ đầu tiên của Xuân Sang
-    + Viết thêm hàm đọc/ghi một người thuê từ file/ra file
+    <t>- Từ tác vụ đầu tiên của Xuân Lam, viết thêm hàm
++ Kiểm tra tài khoản đã tồn tại hay chưa
++ Thêm một người thuê vào danh sách
++ Xuất danh sách người thuê</t>
+  </si>
+  <si>
+    <t>[Viết thêm hàm vào file ThueNhieuMay.hpp]
+- Chỉnh sửa danh sách người thuê, kiểm tra số điện thoại có tồn tại hay không nếu có thì yêu cầu nhập thông tin tài khoản và mật khẩu mới.
+- Xóa một người thuê khỏi danh sách
+- Đọc danh sách người thuê
+- Ghi danh sách người thuê
 [Bổ sung]
-+ Viết thêm hàm thayDoiThongTinTaiKhoanMatKhau()</t>
++ Viết thêm hàm kiểm tra tài khoản, số điện thoại đã tồn tại hay chưa</t>
+  </si>
+  <si>
+    <t>[Tạo mới và viết vào file ThueNhieuMay.hpp]
+- Khai báo dữ liệu danh sách liên kết đơn với  dữ liệu lưu trữ là 1 khách thuê (1 phần tử)
+- Viết các hàm:
++ createList();
++ createNode();
++ addNodeInTail();
++ removeNodeInHead();
++ removeNodeInTail();
++ giaiPhongVungNhoDanhSachNguoiThue();</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Viết thêm hàm vào file ThueNhieuMay.hpp]
+- Ghi danh sách người thuê ra file
+- Xuất danh sách người thuê ra file
+- Tìm kiếm người thuê theo tài khoản
+</t>
+  </si>
+  <si>
+    <t>[Viết thêm hàm vào file ThueNhieuMay.hpp]
+- Tạo một switch case để nhập thông tin muốn chỉnh sửa. VD: 1. Thay đổi tài khoản 2. Thay đổi mật khẩu 3. Thay đổi số điện thoại…</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;Xong&quot;;&quot; &quot;;&quot; &quot;"/>
   </numFmts>
@@ -411,6 +451,18 @@
     <xf numFmtId="164" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -426,21 +478,9 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="49">
     <dxf>
@@ -475,7 +515,6 @@
         <sz val="10"/>
         <color theme="9" tint="-0.499984740745262"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="164" formatCode="&quot;Xong&quot;;&quot; &quot;;&quot; &quot;"/>
@@ -495,7 +534,6 @@
         <sz val="10"/>
         <color theme="1" tint="0.14999847407452621"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <fill>
@@ -552,7 +590,6 @@
         <sz val="10"/>
         <color theme="1" tint="0.14999847407452621"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -571,7 +608,6 @@
         <sz val="10"/>
         <color theme="1" tint="0.14999847407452621"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <fill>
@@ -636,7 +672,6 @@
         <sz val="10"/>
         <color theme="9" tint="-0.499984740745262"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="164" formatCode="&quot;Xong&quot;;&quot; &quot;;&quot; &quot;"/>
@@ -664,7 +699,6 @@
         <sz val="10"/>
         <color theme="1" tint="0.14999847407452621"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <fill>
@@ -729,7 +763,6 @@
         <sz val="10"/>
         <color theme="1" tint="0.14999847407452621"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -756,7 +789,6 @@
         <sz val="10"/>
         <color theme="1" tint="0.14999847407452621"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <fill>
@@ -813,7 +845,6 @@
         <sz val="10"/>
         <color theme="9" tint="-0.499984740745262"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="164" formatCode="&quot;Xong&quot;;&quot; &quot;;&quot; &quot;"/>
@@ -833,7 +864,6 @@
         <sz val="10"/>
         <color theme="1" tint="0.14999847407452621"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <fill>
@@ -890,7 +920,6 @@
         <sz val="10"/>
         <color theme="1" tint="0.14999847407452621"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -909,7 +938,6 @@
         <sz val="10"/>
         <color theme="1" tint="0.14999847407452621"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <fill>
@@ -974,7 +1002,6 @@
         <sz val="10"/>
         <color theme="9" tint="-0.499984740745262"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="164" formatCode="&quot;Xong&quot;;&quot; &quot;;&quot; &quot;"/>
@@ -1002,7 +1029,6 @@
         <sz val="10"/>
         <color theme="1" tint="0.14999847407452621"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <fill>
@@ -1067,7 +1093,6 @@
         <sz val="10"/>
         <color theme="1" tint="0.14999847407452621"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1094,7 +1119,6 @@
         <sz val="10"/>
         <color theme="1" tint="0.14999847407452621"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <fill>
@@ -1151,7 +1175,6 @@
         <sz val="10"/>
         <color theme="9" tint="-0.499984740745262"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="164" formatCode="&quot;Xong&quot;;&quot; &quot;;&quot; &quot;"/>
@@ -1171,7 +1194,6 @@
         <sz val="10"/>
         <color theme="1" tint="0.14999847407452621"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <fill>
@@ -1228,7 +1250,6 @@
         <sz val="10"/>
         <color theme="1" tint="0.14999847407452621"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1247,7 +1268,6 @@
         <sz val="10"/>
         <color theme="1" tint="0.14999847407452621"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <fill>
@@ -1312,7 +1332,6 @@
         <sz val="10"/>
         <color theme="9" tint="-0.499984740745262"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="164" formatCode="&quot;Xong&quot;;&quot; &quot;;&quot; &quot;"/>
@@ -1340,7 +1359,6 @@
         <sz val="10"/>
         <color theme="1" tint="0.14999847407452621"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <fill>
@@ -1397,7 +1415,6 @@
         <sz val="10"/>
         <color theme="1" tint="0.14999847407452621"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1416,7 +1433,6 @@
         <sz val="10"/>
         <color theme="1" tint="0.14999847407452621"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <fill>
@@ -1481,7 +1497,6 @@
         <sz val="10"/>
         <color theme="9" tint="-0.499984740745262"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="164" formatCode="&quot;Xong&quot;;&quot; &quot;;&quot; &quot;"/>
@@ -1501,7 +1516,6 @@
         <sz val="10"/>
         <color theme="1" tint="0.14999847407452621"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <fill>
@@ -1558,7 +1572,6 @@
         <sz val="10"/>
         <color theme="1" tint="0.14999847407452621"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1577,7 +1590,6 @@
         <sz val="10"/>
         <color theme="1" tint="0.14999847407452621"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <fill>
@@ -1634,7 +1646,6 @@
         <sz val="14"/>
         <color theme="1" tint="0.14999847407452621"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1653,7 +1664,6 @@
         <sz val="10"/>
         <color theme="1" tint="0.14999847407452621"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <fill>
@@ -1686,7 +1696,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1704,7 +1713,6 @@
         <sz val="10"/>
         <color theme="1" tint="0.14999847407452621"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1730,7 +1738,6 @@
         <sz val="10"/>
         <color theme="1" tint="0.14999847407452621"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <fill>
@@ -1765,23 +1772,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4F8DC004-656E-4861-8A9B-0664EF57AC8E}" name="Table_Schedule" displayName="Table_Schedule" ref="A12:O28" headerRowCount="0" headerRowDxfId="48" dataDxfId="46" totalsRowDxfId="45" headerRowBorderDxfId="47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_Schedule" displayName="Table_Schedule" ref="A12:O28" headerRowCount="0" headerRowDxfId="48" dataDxfId="46" totalsRowDxfId="45" headerRowBorderDxfId="47">
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{806ED6B8-8ACD-4379-BEDB-96271853BE60}" name="Tác vụ" totalsRowLabel="Tổng" headerRowDxfId="44" dataDxfId="43" totalsRowDxfId="42"/>
-    <tableColumn id="2" xr3:uid="{76033DF7-8A4F-4FEC-A9D7-5C96DCD65545}" name="Đối tượng" headerRowDxfId="41" dataDxfId="40" totalsRowDxfId="39"/>
-    <tableColumn id="3" xr3:uid="{FC475856-1ADC-4916-928A-1299AA6E20FD}" name="Xong" headerRowDxfId="38" dataDxfId="37" totalsRowDxfId="36"/>
-    <tableColumn id="4" xr3:uid="{EA17B5B7-05CA-49DC-931B-18A33B351217}" name="Đối tượng " headerRowDxfId="35" dataDxfId="34" totalsRowDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{097445D5-CCAE-4271-BA40-D77B38F7EAC4}" name="Xong " headerRowDxfId="32" dataDxfId="31" totalsRowDxfId="30"/>
-    <tableColumn id="6" xr3:uid="{26A529CF-159E-4510-94B8-9FDF50A3DF4F}" name="Đối tượng  " headerRowDxfId="29" dataDxfId="28" totalsRowDxfId="27"/>
-    <tableColumn id="7" xr3:uid="{03CA8AD7-F18D-4580-B309-282AF1A68B91}" name="Xong  " headerRowDxfId="26" dataDxfId="25" totalsRowDxfId="24"/>
-    <tableColumn id="8" xr3:uid="{33CAEFAA-1542-47AB-87B3-C4B9695EC426}" name="Đối tượng   " headerRowDxfId="23" dataDxfId="22" totalsRowDxfId="21"/>
-    <tableColumn id="9" xr3:uid="{3CF24C87-317D-4F05-AE74-19845A08F558}" name="Xong   " headerRowDxfId="20" dataDxfId="19" totalsRowDxfId="18"/>
-    <tableColumn id="10" xr3:uid="{370BC611-3BE0-4AA1-B083-EE2263D56D7A}" name="Đối tượng    " headerRowDxfId="17" dataDxfId="16" totalsRowDxfId="15"/>
-    <tableColumn id="11" xr3:uid="{6CEE4BE1-C72C-4F1E-BD2F-855B53B069AB}" name="Xong    " headerRowDxfId="14" dataDxfId="13" totalsRowDxfId="12"/>
-    <tableColumn id="12" xr3:uid="{12477CC1-B017-423F-B819-0CF08ACBB9FD}" name="Đối tượng     " headerRowDxfId="11" dataDxfId="10" totalsRowDxfId="9"/>
-    <tableColumn id="13" xr3:uid="{103F5BE6-9BC6-4696-B197-A49C1461E0FC}" name="Xong     " headerRowDxfId="8" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="14" xr3:uid="{98F43600-3554-4A5E-B6A6-1A278ACAD19E}" name="Đối tượng      " headerRowDxfId="5" dataDxfId="4" totalsRowDxfId="3"/>
-    <tableColumn id="15" xr3:uid="{75F408CF-2E49-434C-BCAC-CC8FBE307CDC}" name="Xong      " totalsRowFunction="count" headerRowDxfId="2" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="1" name="Tác vụ" totalsRowLabel="Tổng" headerRowDxfId="44" dataDxfId="43" totalsRowDxfId="42"/>
+    <tableColumn id="2" name="Đối tượng" headerRowDxfId="41" dataDxfId="40" totalsRowDxfId="39"/>
+    <tableColumn id="3" name="Xong" headerRowDxfId="38" dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="4" name="Đối tượng " headerRowDxfId="35" dataDxfId="34" totalsRowDxfId="33"/>
+    <tableColumn id="5" name="Xong " headerRowDxfId="32" dataDxfId="31" totalsRowDxfId="30"/>
+    <tableColumn id="6" name="Đối tượng  " headerRowDxfId="29" dataDxfId="28" totalsRowDxfId="27"/>
+    <tableColumn id="7" name="Xong  " headerRowDxfId="26" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="8" name="Đối tượng   " headerRowDxfId="23" dataDxfId="22" totalsRowDxfId="21"/>
+    <tableColumn id="9" name="Xong   " headerRowDxfId="20" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="10" name="Đối tượng    " headerRowDxfId="17" dataDxfId="16" totalsRowDxfId="15"/>
+    <tableColumn id="11" name="Xong    " headerRowDxfId="14" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="12" name="Đối tượng     " headerRowDxfId="11" dataDxfId="10" totalsRowDxfId="9"/>
+    <tableColumn id="13" name="Xong     " headerRowDxfId="8" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="14" name="Đối tượng      " headerRowDxfId="5" dataDxfId="4" totalsRowDxfId="3"/>
+    <tableColumn id="15" name="Xong      " totalsRowFunction="count" headerRowDxfId="2" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2083,221 +2090,221 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ACBE16D-A30F-4C6E-8649-E8A1F3FD2B44}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="62.6640625" style="1" customWidth="1"/>
-    <col min="2" max="15" width="12.77734375" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="62.7109375" style="1" customWidth="1"/>
+    <col min="2" max="15" width="12.7109375" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="18"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="18"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="18"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="18"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="18"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="18"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="18"/>
     </row>
-    <row r="9" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="17" t="s">
+      <c r="C9" s="20"/>
+      <c r="D9" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="18" t="s">
+      <c r="E9" s="20"/>
+      <c r="F9" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="18"/>
-      <c r="H9" s="17" t="s">
+      <c r="G9" s="22"/>
+      <c r="H9" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="16"/>
-      <c r="J9" s="18" t="s">
+      <c r="I9" s="20"/>
+      <c r="J9" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="18"/>
-      <c r="L9" s="17" t="s">
+      <c r="K9" s="22"/>
+      <c r="L9" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="M9" s="16"/>
-      <c r="N9" s="17" t="s">
+      <c r="M9" s="20"/>
+      <c r="N9" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="O9" s="18"/>
+      <c r="O9" s="22"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
-      <c r="B10" s="21">
+      <c r="B10" s="16">
         <v>44814</v>
       </c>
-      <c r="C10" s="22"/>
-      <c r="D10" s="19">
+      <c r="C10" s="17"/>
+      <c r="D10" s="14">
         <v>44844</v>
       </c>
-      <c r="E10" s="22"/>
-      <c r="F10" s="20">
+      <c r="E10" s="17"/>
+      <c r="F10" s="15">
         <v>44875</v>
       </c>
-      <c r="G10" s="20"/>
-      <c r="H10" s="19">
+      <c r="G10" s="15"/>
+      <c r="H10" s="14">
         <v>44905</v>
       </c>
-      <c r="I10" s="22"/>
-      <c r="J10" s="20" t="s">
+      <c r="I10" s="17"/>
+      <c r="J10" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="K10" s="20"/>
-      <c r="L10" s="19" t="s">
+      <c r="K10" s="15"/>
+      <c r="L10" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="M10" s="22"/>
-      <c r="N10" s="19" t="s">
+      <c r="M10" s="17"/>
+      <c r="N10" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="O10" s="20"/>
+      <c r="O10" s="15"/>
     </row>
-    <row r="11" spans="1:15" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>1</v>
       </c>
@@ -2320,9 +2327,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="261.60000000000002" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="288.75" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>15</v>
@@ -2345,9 +2352,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="137.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="137.44999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>16</v>
@@ -2370,7 +2377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="49.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="49.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
         <v>17</v>
       </c>
@@ -2393,7 +2400,7 @@
       <c r="N14" s="10"/>
       <c r="O14" s="11"/>
     </row>
-    <row r="15" spans="1:15" ht="70.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
         <v>19</v>
       </c>
@@ -2416,11 +2423,15 @@
       <c r="N15" s="10"/>
       <c r="O15" s="11"/>
     </row>
-    <row r="16" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
+    <row r="16" spans="1:15" ht="201" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
+        <v>25</v>
+      </c>
       <c r="B16" s="10"/>
       <c r="C16" s="11"/>
-      <c r="D16" s="12"/>
+      <c r="D16" s="12" t="s">
+        <v>21</v>
+      </c>
       <c r="E16" s="13"/>
       <c r="F16" s="10"/>
       <c r="G16" s="11"/>
@@ -2433,11 +2444,15 @@
       <c r="N16" s="10"/>
       <c r="O16" s="11"/>
     </row>
-    <row r="17" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
+    <row r="17" spans="1:15" ht="83.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="B17" s="10"/>
       <c r="C17" s="11"/>
-      <c r="D17" s="12"/>
+      <c r="D17" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="E17" s="13"/>
       <c r="F17" s="10"/>
       <c r="G17" s="11"/>
@@ -2450,11 +2465,15 @@
       <c r="N17" s="10"/>
       <c r="O17" s="11"/>
     </row>
-    <row r="18" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
+    <row r="18" spans="1:15" ht="200.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="9" t="s">
+        <v>24</v>
+      </c>
       <c r="B18" s="10"/>
       <c r="C18" s="11"/>
-      <c r="D18" s="12"/>
+      <c r="D18" s="12" t="s">
+        <v>4</v>
+      </c>
       <c r="E18" s="13"/>
       <c r="F18" s="10"/>
       <c r="G18" s="11"/>
@@ -2467,11 +2486,15 @@
       <c r="N18" s="10"/>
       <c r="O18" s="11"/>
     </row>
-    <row r="19" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
+    <row r="19" spans="1:15" ht="81.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="9" t="s">
+        <v>26</v>
+      </c>
       <c r="B19" s="10"/>
       <c r="C19" s="11"/>
-      <c r="D19" s="12"/>
+      <c r="D19" s="12" t="s">
+        <v>15</v>
+      </c>
       <c r="E19" s="13"/>
       <c r="F19" s="10"/>
       <c r="G19" s="11"/>
@@ -2484,11 +2507,15 @@
       <c r="N19" s="10"/>
       <c r="O19" s="11"/>
     </row>
-    <row r="20" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
+    <row r="20" spans="1:15" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="9" t="s">
+        <v>27</v>
+      </c>
       <c r="B20" s="10"/>
       <c r="C20" s="11"/>
-      <c r="D20" s="12"/>
+      <c r="D20" s="12" t="s">
+        <v>16</v>
+      </c>
       <c r="E20" s="13"/>
       <c r="F20" s="10"/>
       <c r="G20" s="11"/>
@@ -2501,7 +2528,7 @@
       <c r="N20" s="10"/>
       <c r="O20" s="11"/>
     </row>
-    <row r="21" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" s="9"/>
       <c r="B21" s="10"/>
       <c r="C21" s="11"/>
@@ -2518,7 +2545,7 @@
       <c r="N21" s="10"/>
       <c r="O21" s="11"/>
     </row>
-    <row r="22" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" s="9"/>
       <c r="B22" s="10"/>
       <c r="C22" s="11"/>
@@ -2535,7 +2562,7 @@
       <c r="N22" s="10"/>
       <c r="O22" s="11"/>
     </row>
-    <row r="23" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" s="9"/>
       <c r="B23" s="10"/>
       <c r="C23" s="11"/>
@@ -2552,7 +2579,7 @@
       <c r="N23" s="10"/>
       <c r="O23" s="11"/>
     </row>
-    <row r="24" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" s="9"/>
       <c r="B24" s="10"/>
       <c r="C24" s="11"/>
@@ -2569,7 +2596,7 @@
       <c r="N24" s="10"/>
       <c r="O24" s="11"/>
     </row>
-    <row r="25" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" s="9"/>
       <c r="B25" s="10"/>
       <c r="C25" s="11"/>
@@ -2586,7 +2613,7 @@
       <c r="N25" s="10"/>
       <c r="O25" s="11"/>
     </row>
-    <row r="26" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" s="9"/>
       <c r="B26" s="10"/>
       <c r="C26" s="11"/>
@@ -2603,7 +2630,7 @@
       <c r="N26" s="10"/>
       <c r="O26" s="11"/>
     </row>
-    <row r="27" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" s="9"/>
       <c r="B27" s="10"/>
       <c r="C27" s="11"/>
@@ -2620,7 +2647,7 @@
       <c r="N27" s="10"/>
       <c r="O27" s="11"/>
     </row>
-    <row r="28" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" s="9"/>
       <c r="B28" s="10"/>
       <c r="C28" s="11"/>
@@ -2639,13 +2666,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="L10:M10"/>
     <mergeCell ref="A1:O8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="D9:E9"/>
@@ -2654,18 +2674,25 @@
     <mergeCell ref="J9:K9"/>
     <mergeCell ref="L9:M9"/>
     <mergeCell ref="N9:O9"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="L10:M10"/>
   </mergeCells>
   <dataValidations count="10">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Nhập ngày đầu tiên trong tuần đối với lịch biểu việc nhà." sqref="B10" xr:uid="{3049090B-60E9-4942-8275-FDD8077FACF7}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Trong cột này, nhập tên của người được chỉ định cho từng nhiệm vụ làm việc nhà trong Ngày 1." sqref="B11" xr:uid="{CC4CF256-97B4-4044-AD35-849B6B830DD5}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Trong cột này, nhập tên của người được chỉ định cho từng nhiệm vụ làm việc nhà trong Ngày 2." sqref="D11" xr:uid="{1982495C-D7A9-40B1-ADD2-943E33D1C3B6}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Trong cột này, nhập tên của người được chỉ định cho từng nhiệm vụ làm việc nhà trong Ngày 3." sqref="F11" xr:uid="{6B8A2A3A-59CD-4FC8-9259-1FCA6B85E69E}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Trong cột này, nhập tên của người được chỉ định cho từng nhiệm vụ làm việc nhà trong Ngày 4." sqref="H11" xr:uid="{709B72C2-3E0F-4075-87BD-12774E0A737C}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Trong cột này, nhập tên của người được chỉ định cho từng nhiệm vụ làm việc nhà trong Ngày 5." sqref="J11" xr:uid="{BBA1D69A-4EF6-40D7-B671-B274C473A753}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Trong cột này, nhập tên của người được chỉ định cho từng nhiệm vụ làm việc nhà trong Ngày 6." sqref="L11" xr:uid="{BB3701CE-3B67-4B7A-8FEC-E11CC151F503}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Bấm đúp vào ô bên dưới cột này để đánh dấu nhiệm vụ là đã hoàn thành." sqref="E11 G11 I11 K11 M11 O11 C11" xr:uid="{DAE6333A-D931-4FBE-A8DE-2FAF955BE2C3}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Nhập mỗi nhiệm vụ làm việc nhà trong cột này." sqref="A11" xr:uid="{D8426EEE-6D9B-403C-8FD8-36E87418C774}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Trong cột này, nhập tên của người được chỉ định cho từng nhiệm vụ làm việc nhà trong Ngày 7." sqref="N11" xr:uid="{935CB533-5DDA-42D3-B262-8558CD722DF7}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Nhập ngày đầu tiên trong tuần đối với lịch biểu việc nhà." sqref="B10"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Trong cột này, nhập tên của người được chỉ định cho từng nhiệm vụ làm việc nhà trong Ngày 1." sqref="B11"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Trong cột này, nhập tên của người được chỉ định cho từng nhiệm vụ làm việc nhà trong Ngày 2." sqref="D11"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Trong cột này, nhập tên của người được chỉ định cho từng nhiệm vụ làm việc nhà trong Ngày 3." sqref="F11"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Trong cột này, nhập tên của người được chỉ định cho từng nhiệm vụ làm việc nhà trong Ngày 4." sqref="H11"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Trong cột này, nhập tên của người được chỉ định cho từng nhiệm vụ làm việc nhà trong Ngày 5." sqref="J11"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Trong cột này, nhập tên của người được chỉ định cho từng nhiệm vụ làm việc nhà trong Ngày 6." sqref="L11"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Bấm đúp vào ô bên dưới cột này để đánh dấu nhiệm vụ là đã hoàn thành." sqref="E11 G11 I11 K11 M11 O11 C11"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Nhập mỗi nhiệm vụ làm việc nhà trong cột này." sqref="A11"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Trong cột này, nhập tên của người được chỉ định cho từng nhiệm vụ làm việc nhà trong Ngày 7." sqref="N11"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
cập nhật kế hoạch phân công tuần 3 (12/10/22)
cập nhật kế hoạch phân công tuần 3 (12/10/22)
</commit_message>
<xml_diff>
--- a/plan/kehoachphancong_tuan3.xlsx
+++ b/plan/kehoachphancong_tuan3.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\comeh\Documents\GitHub\Do_An_Quan_Ly_Phong_Game\plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E59C03-201E-4A12-A136-ED054A14967C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Trang_tính1" sheetId="1" r:id="rId1"/>
@@ -21,17 +22,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -164,7 +154,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;Xong&quot;;&quot; &quot;;&quot; &quot;"/>
   </numFmts>
@@ -451,18 +441,6 @@
     <xf numFmtId="164" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -478,9 +456,21 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="49">
     <dxf>
@@ -1772,23 +1762,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_Schedule" displayName="Table_Schedule" ref="A12:O28" headerRowCount="0" headerRowDxfId="48" dataDxfId="46" totalsRowDxfId="45" headerRowBorderDxfId="47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_Schedule" displayName="Table_Schedule" ref="A12:O28" headerRowCount="0" headerRowDxfId="48" dataDxfId="46" totalsRowDxfId="45" headerRowBorderDxfId="47">
   <tableColumns count="15">
-    <tableColumn id="1" name="Tác vụ" totalsRowLabel="Tổng" headerRowDxfId="44" dataDxfId="43" totalsRowDxfId="42"/>
-    <tableColumn id="2" name="Đối tượng" headerRowDxfId="41" dataDxfId="40" totalsRowDxfId="39"/>
-    <tableColumn id="3" name="Xong" headerRowDxfId="38" dataDxfId="37" totalsRowDxfId="36"/>
-    <tableColumn id="4" name="Đối tượng " headerRowDxfId="35" dataDxfId="34" totalsRowDxfId="33"/>
-    <tableColumn id="5" name="Xong " headerRowDxfId="32" dataDxfId="31" totalsRowDxfId="30"/>
-    <tableColumn id="6" name="Đối tượng  " headerRowDxfId="29" dataDxfId="28" totalsRowDxfId="27"/>
-    <tableColumn id="7" name="Xong  " headerRowDxfId="26" dataDxfId="25" totalsRowDxfId="24"/>
-    <tableColumn id="8" name="Đối tượng   " headerRowDxfId="23" dataDxfId="22" totalsRowDxfId="21"/>
-    <tableColumn id="9" name="Xong   " headerRowDxfId="20" dataDxfId="19" totalsRowDxfId="18"/>
-    <tableColumn id="10" name="Đối tượng    " headerRowDxfId="17" dataDxfId="16" totalsRowDxfId="15"/>
-    <tableColumn id="11" name="Xong    " headerRowDxfId="14" dataDxfId="13" totalsRowDxfId="12"/>
-    <tableColumn id="12" name="Đối tượng     " headerRowDxfId="11" dataDxfId="10" totalsRowDxfId="9"/>
-    <tableColumn id="13" name="Xong     " headerRowDxfId="8" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="14" name="Đối tượng      " headerRowDxfId="5" dataDxfId="4" totalsRowDxfId="3"/>
-    <tableColumn id="15" name="Xong      " totalsRowFunction="count" headerRowDxfId="2" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Tác vụ" totalsRowLabel="Tổng" headerRowDxfId="44" dataDxfId="43" totalsRowDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Đối tượng" headerRowDxfId="41" dataDxfId="40" totalsRowDxfId="39"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Xong" headerRowDxfId="38" dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Đối tượng " headerRowDxfId="35" dataDxfId="34" totalsRowDxfId="33"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Xong " headerRowDxfId="32" dataDxfId="31" totalsRowDxfId="30"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Đối tượng  " headerRowDxfId="29" dataDxfId="28" totalsRowDxfId="27"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Xong  " headerRowDxfId="26" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Đối tượng   " headerRowDxfId="23" dataDxfId="22" totalsRowDxfId="21"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Xong   " headerRowDxfId="20" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Đối tượng    " headerRowDxfId="17" dataDxfId="16" totalsRowDxfId="15"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Xong    " headerRowDxfId="14" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Đối tượng     " headerRowDxfId="11" dataDxfId="10" totalsRowDxfId="9"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Xong     " headerRowDxfId="8" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Đối tượng      " headerRowDxfId="5" dataDxfId="4" totalsRowDxfId="3"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Xong      " totalsRowFunction="count" headerRowDxfId="2" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2090,221 +2080,221 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="62.7109375" style="1" customWidth="1"/>
-    <col min="2" max="15" width="12.7109375" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="62.6640625" style="1" customWidth="1"/>
+    <col min="2" max="15" width="12.6640625" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="18"/>
-      <c r="O3" s="18"/>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="18"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
-      <c r="N4" s="18"/>
-      <c r="O4" s="18"/>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="18"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="18"/>
-      <c r="O5" s="18"/>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" s="18"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="18"/>
-      <c r="O6" s="18"/>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="14"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="18"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="14"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="18"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
-      <c r="O8" s="18"/>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
     </row>
-    <row r="9" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="21" t="s">
+      <c r="C9" s="16"/>
+      <c r="D9" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="20"/>
-      <c r="F9" s="22" t="s">
+      <c r="E9" s="16"/>
+      <c r="F9" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="22"/>
-      <c r="H9" s="21" t="s">
+      <c r="G9" s="18"/>
+      <c r="H9" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="20"/>
-      <c r="J9" s="22" t="s">
+      <c r="I9" s="16"/>
+      <c r="J9" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="22"/>
-      <c r="L9" s="21" t="s">
+      <c r="K9" s="18"/>
+      <c r="L9" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="M9" s="20"/>
-      <c r="N9" s="21" t="s">
+      <c r="M9" s="16"/>
+      <c r="N9" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="O9" s="22"/>
+      <c r="O9" s="18"/>
     </row>
-    <row r="10" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="16">
+      <c r="B10" s="21">
         <v>44814</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="14">
+      <c r="C10" s="22"/>
+      <c r="D10" s="19">
         <v>44844</v>
       </c>
-      <c r="E10" s="17"/>
-      <c r="F10" s="15">
+      <c r="E10" s="22"/>
+      <c r="F10" s="20">
         <v>44875</v>
       </c>
-      <c r="G10" s="15"/>
-      <c r="H10" s="14">
+      <c r="G10" s="20"/>
+      <c r="H10" s="19">
         <v>44905</v>
       </c>
-      <c r="I10" s="17"/>
-      <c r="J10" s="15" t="s">
+      <c r="I10" s="22"/>
+      <c r="J10" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="K10" s="15"/>
-      <c r="L10" s="14" t="s">
+      <c r="K10" s="20"/>
+      <c r="L10" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="M10" s="17"/>
-      <c r="N10" s="14" t="s">
+      <c r="M10" s="22"/>
+      <c r="N10" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="O10" s="15"/>
+      <c r="O10" s="20"/>
     </row>
-    <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>1</v>
       </c>
@@ -2327,7 +2317,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="288.75" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" ht="279" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>22</v>
       </c>
@@ -2352,7 +2342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="137.44999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="137.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>20</v>
       </c>
@@ -2377,7 +2367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="49.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" ht="49.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>17</v>
       </c>
@@ -2400,7 +2390,7 @@
       <c r="N14" s="10"/>
       <c r="O14" s="11"/>
     </row>
-    <row r="15" spans="1:15" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="70.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>19</v>
       </c>
@@ -2423,19 +2413,19 @@
       <c r="N15" s="10"/>
       <c r="O15" s="11"/>
     </row>
-    <row r="16" spans="1:15" ht="201" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="201" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>25</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="11"/>
-      <c r="D16" s="12" t="s">
-        <v>21</v>
-      </c>
+      <c r="D16" s="12"/>
       <c r="E16" s="13"/>
       <c r="F16" s="10"/>
       <c r="G16" s="11"/>
-      <c r="H16" s="12"/>
+      <c r="H16" s="12" t="s">
+        <v>21</v>
+      </c>
       <c r="I16" s="13"/>
       <c r="J16" s="10"/>
       <c r="K16" s="11"/>
@@ -2444,19 +2434,19 @@
       <c r="N16" s="10"/>
       <c r="O16" s="11"/>
     </row>
-    <row r="17" spans="1:15" ht="83.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>23</v>
       </c>
       <c r="B17" s="10"/>
       <c r="C17" s="11"/>
-      <c r="D17" s="12" t="s">
-        <v>18</v>
-      </c>
+      <c r="D17" s="12"/>
       <c r="E17" s="13"/>
       <c r="F17" s="10"/>
       <c r="G17" s="11"/>
-      <c r="H17" s="12"/>
+      <c r="H17" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="I17" s="13"/>
       <c r="J17" s="10"/>
       <c r="K17" s="11"/>
@@ -2465,19 +2455,19 @@
       <c r="N17" s="10"/>
       <c r="O17" s="11"/>
     </row>
-    <row r="18" spans="1:15" ht="200.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" ht="200.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>24</v>
       </c>
       <c r="B18" s="10"/>
       <c r="C18" s="11"/>
-      <c r="D18" s="12" t="s">
-        <v>4</v>
-      </c>
+      <c r="D18" s="12"/>
       <c r="E18" s="13"/>
       <c r="F18" s="10"/>
       <c r="G18" s="11"/>
-      <c r="H18" s="12"/>
+      <c r="H18" s="12" t="s">
+        <v>4</v>
+      </c>
       <c r="I18" s="13"/>
       <c r="J18" s="10"/>
       <c r="K18" s="11"/>
@@ -2486,19 +2476,19 @@
       <c r="N18" s="10"/>
       <c r="O18" s="11"/>
     </row>
-    <row r="19" spans="1:15" ht="81.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>26</v>
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="11"/>
-      <c r="D19" s="12" t="s">
-        <v>15</v>
-      </c>
+      <c r="D19" s="12"/>
       <c r="E19" s="13"/>
       <c r="F19" s="10"/>
       <c r="G19" s="11"/>
-      <c r="H19" s="12"/>
+      <c r="H19" s="12" t="s">
+        <v>15</v>
+      </c>
       <c r="I19" s="13"/>
       <c r="J19" s="10"/>
       <c r="K19" s="11"/>
@@ -2507,19 +2497,19 @@
       <c r="N19" s="10"/>
       <c r="O19" s="11"/>
     </row>
-    <row r="20" spans="1:15" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>27</v>
       </c>
       <c r="B20" s="10"/>
       <c r="C20" s="11"/>
-      <c r="D20" s="12" t="s">
-        <v>16</v>
-      </c>
+      <c r="D20" s="12"/>
       <c r="E20" s="13"/>
       <c r="F20" s="10"/>
       <c r="G20" s="11"/>
-      <c r="H20" s="12"/>
+      <c r="H20" s="12" t="s">
+        <v>16</v>
+      </c>
       <c r="I20" s="13"/>
       <c r="J20" s="10"/>
       <c r="K20" s="11"/>
@@ -2528,7 +2518,7 @@
       <c r="N20" s="10"/>
       <c r="O20" s="11"/>
     </row>
-    <row r="21" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
       <c r="B21" s="10"/>
       <c r="C21" s="11"/>
@@ -2545,7 +2535,7 @@
       <c r="N21" s="10"/>
       <c r="O21" s="11"/>
     </row>
-    <row r="22" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
       <c r="B22" s="10"/>
       <c r="C22" s="11"/>
@@ -2562,7 +2552,7 @@
       <c r="N22" s="10"/>
       <c r="O22" s="11"/>
     </row>
-    <row r="23" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
       <c r="B23" s="10"/>
       <c r="C23" s="11"/>
@@ -2579,7 +2569,7 @@
       <c r="N23" s="10"/>
       <c r="O23" s="11"/>
     </row>
-    <row r="24" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
       <c r="B24" s="10"/>
       <c r="C24" s="11"/>
@@ -2596,7 +2586,7 @@
       <c r="N24" s="10"/>
       <c r="O24" s="11"/>
     </row>
-    <row r="25" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
       <c r="B25" s="10"/>
       <c r="C25" s="11"/>
@@ -2613,7 +2603,7 @@
       <c r="N25" s="10"/>
       <c r="O25" s="11"/>
     </row>
-    <row r="26" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
       <c r="B26" s="10"/>
       <c r="C26" s="11"/>
@@ -2630,7 +2620,7 @@
       <c r="N26" s="10"/>
       <c r="O26" s="11"/>
     </row>
-    <row r="27" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
       <c r="B27" s="10"/>
       <c r="C27" s="11"/>
@@ -2647,7 +2637,7 @@
       <c r="N27" s="10"/>
       <c r="O27" s="11"/>
     </row>
-    <row r="28" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
       <c r="B28" s="10"/>
       <c r="C28" s="11"/>
@@ -2666,6 +2656,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="L10:M10"/>
     <mergeCell ref="A1:O8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="D9:E9"/>
@@ -2674,25 +2671,18 @@
     <mergeCell ref="J9:K9"/>
     <mergeCell ref="L9:M9"/>
     <mergeCell ref="N9:O9"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="L10:M10"/>
   </mergeCells>
   <dataValidations count="10">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Nhập ngày đầu tiên trong tuần đối với lịch biểu việc nhà." sqref="B10"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Trong cột này, nhập tên của người được chỉ định cho từng nhiệm vụ làm việc nhà trong Ngày 1." sqref="B11"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Trong cột này, nhập tên của người được chỉ định cho từng nhiệm vụ làm việc nhà trong Ngày 2." sqref="D11"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Trong cột này, nhập tên của người được chỉ định cho từng nhiệm vụ làm việc nhà trong Ngày 3." sqref="F11"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Trong cột này, nhập tên của người được chỉ định cho từng nhiệm vụ làm việc nhà trong Ngày 4." sqref="H11"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Trong cột này, nhập tên của người được chỉ định cho từng nhiệm vụ làm việc nhà trong Ngày 5." sqref="J11"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Trong cột này, nhập tên của người được chỉ định cho từng nhiệm vụ làm việc nhà trong Ngày 6." sqref="L11"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Bấm đúp vào ô bên dưới cột này để đánh dấu nhiệm vụ là đã hoàn thành." sqref="E11 G11 I11 K11 M11 O11 C11"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Nhập mỗi nhiệm vụ làm việc nhà trong cột này." sqref="A11"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Trong cột này, nhập tên của người được chỉ định cho từng nhiệm vụ làm việc nhà trong Ngày 7." sqref="N11"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Nhập ngày đầu tiên trong tuần đối với lịch biểu việc nhà." sqref="B10" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Trong cột này, nhập tên của người được chỉ định cho từng nhiệm vụ làm việc nhà trong Ngày 1." sqref="B11" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Trong cột này, nhập tên của người được chỉ định cho từng nhiệm vụ làm việc nhà trong Ngày 2." sqref="D11" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Trong cột này, nhập tên của người được chỉ định cho từng nhiệm vụ làm việc nhà trong Ngày 3." sqref="F11" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Trong cột này, nhập tên của người được chỉ định cho từng nhiệm vụ làm việc nhà trong Ngày 4." sqref="H11" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Trong cột này, nhập tên của người được chỉ định cho từng nhiệm vụ làm việc nhà trong Ngày 5." sqref="J11" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Trong cột này, nhập tên của người được chỉ định cho từng nhiệm vụ làm việc nhà trong Ngày 6." sqref="L11" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Bấm đúp vào ô bên dưới cột này để đánh dấu nhiệm vụ là đã hoàn thành." sqref="E11 G11 I11 K11 M11 O11 C11" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Nhập mỗi nhiệm vụ làm việc nhà trong cột này." sqref="A11" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Trong cột này, nhập tên của người được chỉ định cho từng nhiệm vụ làm việc nhà trong Ngày 7." sqref="N11" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
viet code theo phan cong
viet code theo phan cong
</commit_message>
<xml_diff>
--- a/plan/kehoachphancong_tuan3.xlsx
+++ b/plan/kehoachphancong_tuan3.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\comeh\Documents\GitHub\DOAN\xuanlam\Do_An_Quan_Ly_Phong_Game\plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\comeh\Documents\GitHub\Do_An_Quan_Ly_Phong_Game\plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF6F1B08-AB97-451C-9A38-AF6925D6CEA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E59C03-201E-4A12-A136-ED054A14967C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -441,18 +441,6 @@
     <xf numFmtId="164" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -466,6 +454,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2084,7 +2084,7 @@
   <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2095,204 +2095,204 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="18"/>
-      <c r="O3" s="18"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
-      <c r="N4" s="18"/>
-      <c r="O4" s="18"/>
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="18"/>
-      <c r="O5" s="18"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="18"/>
-      <c r="O6" s="18"/>
+      <c r="A6" s="14"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
+      <c r="A7" s="14"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
-      <c r="O8" s="18"/>
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
     </row>
     <row r="9" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="21" t="s">
+      <c r="C9" s="16"/>
+      <c r="D9" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="20"/>
-      <c r="F9" s="22" t="s">
+      <c r="E9" s="16"/>
+      <c r="F9" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="22"/>
-      <c r="H9" s="21" t="s">
+      <c r="G9" s="18"/>
+      <c r="H9" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="20"/>
-      <c r="J9" s="22" t="s">
+      <c r="I9" s="16"/>
+      <c r="J9" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="22"/>
-      <c r="L9" s="21" t="s">
+      <c r="K9" s="18"/>
+      <c r="L9" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="M9" s="20"/>
-      <c r="N9" s="21" t="s">
+      <c r="M9" s="16"/>
+      <c r="N9" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="O9" s="22"/>
+      <c r="O9" s="18"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="16">
+      <c r="B10" s="21">
         <v>44814</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="14">
+      <c r="C10" s="22"/>
+      <c r="D10" s="19">
         <v>44844</v>
       </c>
-      <c r="E10" s="17"/>
-      <c r="F10" s="15">
+      <c r="E10" s="22"/>
+      <c r="F10" s="20">
         <v>44875</v>
       </c>
-      <c r="G10" s="15"/>
-      <c r="H10" s="14">
+      <c r="G10" s="20"/>
+      <c r="H10" s="19">
         <v>44905</v>
       </c>
-      <c r="I10" s="17"/>
-      <c r="J10" s="15" t="s">
+      <c r="I10" s="22"/>
+      <c r="J10" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="K10" s="15"/>
-      <c r="L10" s="14" t="s">
+      <c r="K10" s="20"/>
+      <c r="L10" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="M10" s="17"/>
-      <c r="N10" s="14" t="s">
+      <c r="M10" s="22"/>
+      <c r="N10" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="O10" s="15"/>
+      <c r="O10" s="20"/>
     </row>
     <row r="11" spans="1:15" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
@@ -2426,9 +2426,7 @@
       <c r="H16" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="I16" s="13">
-        <v>1</v>
-      </c>
+      <c r="I16" s="13"/>
       <c r="J16" s="10"/>
       <c r="K16" s="11"/>
       <c r="L16" s="12"/>
@@ -2658,6 +2656,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="L10:M10"/>
     <mergeCell ref="A1:O8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="D9:E9"/>
@@ -2666,13 +2671,6 @@
     <mergeCell ref="J9:K9"/>
     <mergeCell ref="L9:M9"/>
     <mergeCell ref="N9:O9"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="L10:M10"/>
   </mergeCells>
   <dataValidations count="10">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Nhập ngày đầu tiên trong tuần đối với lịch biểu việc nhà." sqref="B10" xr:uid="{00000000-0002-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Viết code theo phân công
Viết code theo phân công
</commit_message>
<xml_diff>
--- a/plan/kehoachphancong_tuan3.xlsx
+++ b/plan/kehoachphancong_tuan3.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\comeh\Documents\GitHub\DOAN\haison\Do_An_Quan_Ly_Phong_Game\plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\comeh\Documents\GitHub\Do_An_Quan_Ly_Phong_Game\plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4628717-40D7-41A8-A7AF-65095A0F0706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A435A7D6-8252-44A0-8B32-2D6D005EC41D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3768" yWindow="2088" windowWidth="17280" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -441,18 +441,6 @@
     <xf numFmtId="164" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -466,6 +454,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2083,8 +2083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2095,204 +2095,204 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="18"/>
-      <c r="O3" s="18"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
-      <c r="N4" s="18"/>
-      <c r="O4" s="18"/>
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="18"/>
-      <c r="O5" s="18"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="18"/>
-      <c r="O6" s="18"/>
+      <c r="A6" s="14"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
+      <c r="A7" s="14"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
-      <c r="O8" s="18"/>
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
     </row>
     <row r="9" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="21" t="s">
+      <c r="C9" s="16"/>
+      <c r="D9" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="20"/>
-      <c r="F9" s="22" t="s">
+      <c r="E9" s="16"/>
+      <c r="F9" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="22"/>
-      <c r="H9" s="21" t="s">
+      <c r="G9" s="18"/>
+      <c r="H9" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="20"/>
-      <c r="J9" s="22" t="s">
+      <c r="I9" s="16"/>
+      <c r="J9" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="22"/>
-      <c r="L9" s="21" t="s">
+      <c r="K9" s="18"/>
+      <c r="L9" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="M9" s="20"/>
-      <c r="N9" s="21" t="s">
+      <c r="M9" s="16"/>
+      <c r="N9" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="O9" s="22"/>
+      <c r="O9" s="18"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="16">
+      <c r="B10" s="21">
         <v>44814</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="14">
+      <c r="C10" s="22"/>
+      <c r="D10" s="19">
         <v>44844</v>
       </c>
-      <c r="E10" s="17"/>
-      <c r="F10" s="15">
+      <c r="E10" s="22"/>
+      <c r="F10" s="20">
         <v>44875</v>
       </c>
-      <c r="G10" s="15"/>
-      <c r="H10" s="14">
+      <c r="G10" s="20"/>
+      <c r="H10" s="19">
         <v>44905</v>
       </c>
-      <c r="I10" s="17"/>
-      <c r="J10" s="15" t="s">
+      <c r="I10" s="22"/>
+      <c r="J10" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="K10" s="15"/>
-      <c r="L10" s="14" t="s">
+      <c r="K10" s="20"/>
+      <c r="L10" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="M10" s="17"/>
-      <c r="N10" s="14" t="s">
+      <c r="M10" s="22"/>
+      <c r="N10" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="O10" s="15"/>
+      <c r="O10" s="20"/>
     </row>
     <row r="11" spans="1:15" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
@@ -2472,7 +2472,9 @@
       <c r="H18" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I18" s="13"/>
+      <c r="I18" s="13">
+        <v>1</v>
+      </c>
       <c r="J18" s="10"/>
       <c r="K18" s="11"/>
       <c r="L18" s="12"/>
@@ -2660,6 +2662,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="L10:M10"/>
     <mergeCell ref="A1:O8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="D9:E9"/>
@@ -2668,13 +2677,6 @@
     <mergeCell ref="J9:K9"/>
     <mergeCell ref="L9:M9"/>
     <mergeCell ref="N9:O9"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="L10:M10"/>
   </mergeCells>
   <dataValidations count="10">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Nhập ngày đầu tiên trong tuần đối với lịch biểu việc nhà." sqref="B10" xr:uid="{00000000-0002-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
viet ham theo phan cong
viet ham theo phan cong
</commit_message>
<xml_diff>
--- a/plan/kehoachphancong_tuan3.xlsx
+++ b/plan/kehoachphancong_tuan3.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\comeh\Documents\GitHub\Do_An_Quan_Ly_Phong_Game\plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\comeh\Documents\GitHub\DOAN\xuansang\Do_An_Quan_Ly_Phong_Game\plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A435A7D6-8252-44A0-8B32-2D6D005EC41D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58067551-7425-40F7-98A6-D9B6CE1D89A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3768" yWindow="2088" windowWidth="17280" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -441,6 +441,18 @@
     <xf numFmtId="164" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -454,18 +466,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2084,7 +2084,7 @@
   <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2095,204 +2095,204 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="18"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="18"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
+      <c r="A6" s="18"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
+      <c r="A7" s="18"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="18"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
+      <c r="A8" s="18"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="18"/>
     </row>
     <row r="9" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="17" t="s">
+      <c r="C9" s="20"/>
+      <c r="D9" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="18" t="s">
+      <c r="E9" s="20"/>
+      <c r="F9" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="18"/>
-      <c r="H9" s="17" t="s">
+      <c r="G9" s="22"/>
+      <c r="H9" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="16"/>
-      <c r="J9" s="18" t="s">
+      <c r="I9" s="20"/>
+      <c r="J9" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="18"/>
-      <c r="L9" s="17" t="s">
+      <c r="K9" s="22"/>
+      <c r="L9" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="M9" s="16"/>
-      <c r="N9" s="17" t="s">
+      <c r="M9" s="20"/>
+      <c r="N9" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="O9" s="18"/>
+      <c r="O9" s="22"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="21">
+      <c r="B10" s="16">
         <v>44814</v>
       </c>
-      <c r="C10" s="22"/>
-      <c r="D10" s="19">
+      <c r="C10" s="17"/>
+      <c r="D10" s="14">
         <v>44844</v>
       </c>
-      <c r="E10" s="22"/>
-      <c r="F10" s="20">
+      <c r="E10" s="17"/>
+      <c r="F10" s="15">
         <v>44875</v>
       </c>
-      <c r="G10" s="20"/>
-      <c r="H10" s="19">
+      <c r="G10" s="15"/>
+      <c r="H10" s="14">
         <v>44905</v>
       </c>
-      <c r="I10" s="22"/>
-      <c r="J10" s="20" t="s">
+      <c r="I10" s="17"/>
+      <c r="J10" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="K10" s="20"/>
-      <c r="L10" s="19" t="s">
+      <c r="K10" s="15"/>
+      <c r="L10" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="M10" s="22"/>
-      <c r="N10" s="19" t="s">
+      <c r="M10" s="17"/>
+      <c r="N10" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="O10" s="20"/>
+      <c r="O10" s="15"/>
     </row>
     <row r="11" spans="1:15" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
@@ -2495,7 +2495,9 @@
       <c r="H19" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="I19" s="13"/>
+      <c r="I19" s="13">
+        <v>1</v>
+      </c>
       <c r="J19" s="10"/>
       <c r="K19" s="11"/>
       <c r="L19" s="12"/>
@@ -2662,13 +2664,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="L10:M10"/>
     <mergeCell ref="A1:O8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="D9:E9"/>
@@ -2677,6 +2672,13 @@
     <mergeCell ref="J9:K9"/>
     <mergeCell ref="L9:M9"/>
     <mergeCell ref="N9:O9"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="L10:M10"/>
   </mergeCells>
   <dataValidations count="10">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Nhập ngày đầu tiên trong tuần đối với lịch biểu việc nhà." sqref="B10" xr:uid="{00000000-0002-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Code theo phân công
Code theo phân công
</commit_message>
<xml_diff>
--- a/plan/kehoachphancong_tuan3.xlsx
+++ b/plan/kehoachphancong_tuan3.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\comeh\Documents\GitHub\DOAN\xuansang\Do_An_Quan_Ly_Phong_Game\plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\comeh\Documents\GitHub\DOAN\thanhsang\Do_An_Quan_Ly_Phong_Game\plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58067551-7425-40F7-98A6-D9B6CE1D89A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F55FDD26-10B0-4424-ACA1-3AE28CF8143E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3768" yWindow="2088" windowWidth="17280" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -441,18 +441,6 @@
     <xf numFmtId="164" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -466,6 +454,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2095,204 +2095,204 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="18"/>
-      <c r="O3" s="18"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
-      <c r="N4" s="18"/>
-      <c r="O4" s="18"/>
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="18"/>
-      <c r="O5" s="18"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="18"/>
-      <c r="O6" s="18"/>
+      <c r="A6" s="14"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
+      <c r="A7" s="14"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
-      <c r="O8" s="18"/>
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
     </row>
     <row r="9" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="21" t="s">
+      <c r="C9" s="16"/>
+      <c r="D9" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="20"/>
-      <c r="F9" s="22" t="s">
+      <c r="E9" s="16"/>
+      <c r="F9" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="22"/>
-      <c r="H9" s="21" t="s">
+      <c r="G9" s="18"/>
+      <c r="H9" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="20"/>
-      <c r="J9" s="22" t="s">
+      <c r="I9" s="16"/>
+      <c r="J9" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="22"/>
-      <c r="L9" s="21" t="s">
+      <c r="K9" s="18"/>
+      <c r="L9" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="M9" s="20"/>
-      <c r="N9" s="21" t="s">
+      <c r="M9" s="16"/>
+      <c r="N9" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="O9" s="22"/>
+      <c r="O9" s="18"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="16">
+      <c r="B10" s="21">
         <v>44814</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="14">
+      <c r="C10" s="22"/>
+      <c r="D10" s="19">
         <v>44844</v>
       </c>
-      <c r="E10" s="17"/>
-      <c r="F10" s="15">
+      <c r="E10" s="22"/>
+      <c r="F10" s="20">
         <v>44875</v>
       </c>
-      <c r="G10" s="15"/>
-      <c r="H10" s="14">
+      <c r="G10" s="20"/>
+      <c r="H10" s="19">
         <v>44905</v>
       </c>
-      <c r="I10" s="17"/>
-      <c r="J10" s="15" t="s">
+      <c r="I10" s="22"/>
+      <c r="J10" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="K10" s="15"/>
-      <c r="L10" s="14" t="s">
+      <c r="K10" s="20"/>
+      <c r="L10" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="M10" s="17"/>
-      <c r="N10" s="14" t="s">
+      <c r="M10" s="22"/>
+      <c r="N10" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="O10" s="15"/>
+      <c r="O10" s="20"/>
     </row>
     <row r="11" spans="1:15" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
@@ -2518,7 +2518,9 @@
       <c r="H20" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="I20" s="13"/>
+      <c r="I20" s="13">
+        <v>1</v>
+      </c>
       <c r="J20" s="10"/>
       <c r="K20" s="11"/>
       <c r="L20" s="12"/>
@@ -2664,6 +2666,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="L10:M10"/>
     <mergeCell ref="A1:O8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="D9:E9"/>
@@ -2672,13 +2681,6 @@
     <mergeCell ref="J9:K9"/>
     <mergeCell ref="L9:M9"/>
     <mergeCell ref="N9:O9"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="L10:M10"/>
   </mergeCells>
   <dataValidations count="10">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Nhập ngày đầu tiên trong tuần đối với lịch biểu việc nhà." sqref="B10" xr:uid="{00000000-0002-0000-0000-000000000000}"/>

</xml_diff>